<commit_message>
updated RachelR table template
</commit_message>
<xml_diff>
--- a/tables/RachelR.xlsx
+++ b/tables/RachelR.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Shtucer\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42ED42B4-9A42-44FD-8713-7A052D02ECBC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B758557E-B279-4E4F-9745-60C1F85A1094}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -70,6 +70,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="170" formatCode="\+0;\-0"/>
+  </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -126,7 +129,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -135,6 +138,7 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="170" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -449,7 +453,7 @@
   <dimension ref="A1:J5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -491,7 +495,7 @@
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="F2" s="3"/>
       <c r="G2" s="3"/>
-      <c r="H2" s="3">
+      <c r="H2" s="6">
         <f>G2-F2</f>
         <v>0</v>
       </c>
@@ -522,7 +526,7 @@
         <f>SUM(A:A) / SUM(C:C)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="H5" s="3" t="e">
+      <c r="H5" s="4" t="e">
         <f>SUM(A:A) / J5</f>
         <v>#DIV/0!</v>
       </c>

</xml_diff>